<commit_message>
até o desafio 4 ponto
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -648,7 +648,7 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -944,7 +944,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D73" activeCellId="0" sqref="D73"/>
     </sheetView>
   </sheetViews>
@@ -1728,8 +1728,8 @@
   </sheetPr>
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D84" activeCellId="0" sqref="D84"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2382,11 +2382,11 @@
         <v>90</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="E58" s="0"/>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
       <c r="B59" s="30" t="n">
         <v>1</v>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="E59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
       <c r="B60" s="30" t="n">
         <v>2</v>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="E60" s="0"/>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
       <c r="B61" s="30" t="n">
         <v>3</v>

</xml_diff>